<commit_message>
correct for res/com sf bug
</commit_message>
<xml_diff>
--- a/summary-tables/SummaryTable_Class_wTotals_formatted_Scenario1.xlsx
+++ b/summary-tables/SummaryTable_Class_wTotals_formatted_Scenario1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Centers-Capacity-Tool\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Centers-Capacity-Tool\summary-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239F5195-2BD3-4D33-A53D-0141D1D721EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C688D4-D5C0-46E6-832B-D1D943B7B060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15630" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UnitsDensity" sheetId="1" r:id="rId1"/>
@@ -937,10 +937,13 @@
     <xf numFmtId="3" fontId="16" fillId="35" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="16" fillId="35" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -949,13 +952,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1330,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,10 +1343,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="46" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="48" t="s">
@@ -1355,27 +1355,27 @@
       <c r="E2" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="45" t="s">
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="45" t="s">
+      <c r="J2" s="42"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="46"/>
-      <c r="N2" s="47"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="44"/>
-      <c r="C3" s="42"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="49"/>
-      <c r="E3" s="44"/>
+      <c r="E3" s="45"/>
       <c r="F3" s="35" t="s">
         <v>7</v>
       </c>
@@ -1415,11 +1415,11 @@
       </c>
       <c r="D4" s="30">
         <f>C4/$C$15</f>
-        <v>6.8933482387297197E-3</v>
+        <v>6.8933482396051479E-3</v>
       </c>
       <c r="E4" s="12">
         <f>(H4+K4)/($H$15+$K$15)</f>
-        <v>8.2418984434804804E-2</v>
+        <v>6.5150653780557136E-2</v>
       </c>
       <c r="F4" s="29">
         <f>SummaryTable_Class_wTotals!D2</f>
@@ -1439,11 +1439,11 @@
       </c>
       <c r="J4" s="2">
         <f>SummaryTable_Class_wTotals!H2</f>
-        <v>22800</v>
+        <v>15500</v>
       </c>
       <c r="K4" s="37">
         <f>SummaryTable_Class_wTotals!I2</f>
-        <v>21800</v>
+        <v>14500</v>
       </c>
       <c r="L4" s="29">
         <f>SummaryTable_Class_wTotals!J2</f>
@@ -1451,11 +1451,11 @@
       </c>
       <c r="M4" s="2">
         <f>SummaryTable_Class_wTotals!K2</f>
-        <v>288</v>
+        <v>259</v>
       </c>
       <c r="N4" s="37">
         <f>SummaryTable_Class_wTotals!L2</f>
-        <v>257</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -1469,11 +1469,11 @@
       </c>
       <c r="D5" s="32">
         <f t="shared" ref="D5:D15" si="0">C5/$C$15</f>
-        <v>1.0536352038936632E-2</v>
+        <v>1.0536352040274708E-2</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" ref="E5:E15" si="1">(H5+K5)/($H$15+$K$15)</f>
-        <v>7.0298545547333502E-2</v>
+        <v>5.5599772598067081E-2</v>
       </c>
       <c r="F5" s="31">
         <f>SummaryTable_Class_wTotals!D3</f>
@@ -1493,11 +1493,11 @@
       </c>
       <c r="J5" s="4">
         <f>SummaryTable_Class_wTotals!H3</f>
-        <v>21700</v>
+        <v>15500</v>
       </c>
       <c r="K5" s="38">
         <f>SummaryTable_Class_wTotals!I3</f>
-        <v>18600</v>
+        <v>12400</v>
       </c>
       <c r="L5" s="31">
         <f>SummaryTable_Class_wTotals!J3</f>
@@ -1505,11 +1505,11 @@
       </c>
       <c r="M5" s="4">
         <f>SummaryTable_Class_wTotals!K3</f>
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="N5" s="38">
         <f>SummaryTable_Class_wTotals!L3</f>
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -1523,11 +1523,11 @@
       </c>
       <c r="D6" s="30">
         <f t="shared" si="0"/>
-        <v>8.2331343094467976E-3</v>
+        <v>8.2331343104923727E-3</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="1"/>
-        <v>3.4447563153865782E-2</v>
+        <v>2.8766344513928368E-2</v>
       </c>
       <c r="F6" s="29">
         <f>SummaryTable_Class_wTotals!D4</f>
@@ -1547,11 +1547,11 @@
       </c>
       <c r="J6" s="2">
         <f>SummaryTable_Class_wTotals!H4</f>
-        <v>11700</v>
+        <v>10000</v>
       </c>
       <c r="K6" s="37">
         <f>SummaryTable_Class_wTotals!I4</f>
-        <v>9400</v>
+        <v>7700</v>
       </c>
       <c r="L6" s="29">
         <f>SummaryTable_Class_wTotals!J4</f>
@@ -1559,11 +1559,11 @@
       </c>
       <c r="M6" s="2">
         <f>SummaryTable_Class_wTotals!K4</f>
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="N6" s="37">
         <f>SummaryTable_Class_wTotals!L4</f>
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
@@ -1577,11 +1577,11 @@
       </c>
       <c r="D7" s="32">
         <f t="shared" si="0"/>
-        <v>2.8909850903816151E-2</v>
+        <v>2.8909850907487589E-2</v>
       </c>
       <c r="E7" s="13">
         <f t="shared" si="1"/>
-        <v>6.90227098749681E-2</v>
+        <v>6.1512222853894259E-2</v>
       </c>
       <c r="F7" s="31">
         <f>SummaryTable_Class_wTotals!D5</f>
@@ -1631,11 +1631,11 @@
       </c>
       <c r="D8" s="30">
         <f t="shared" si="0"/>
-        <v>1.4730107028779206E-2</v>
+        <v>1.4730107030649872E-2</v>
       </c>
       <c r="E8" s="12">
         <f t="shared" si="1"/>
-        <v>2.9982138300586884E-2</v>
+        <v>2.6719727117680499E-2</v>
       </c>
       <c r="F8" s="29">
         <f>SummaryTable_Class_wTotals!D6</f>
@@ -1685,11 +1685,11 @@
       </c>
       <c r="D9" s="32">
         <f t="shared" si="0"/>
-        <v>0.2597374465113943</v>
+        <v>0.25973744654437997</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="1"/>
-        <v>0.30186272008165349</v>
+        <v>0.28698123934053438</v>
       </c>
       <c r="F9" s="31">
         <f>SummaryTable_Class_wTotals!D7</f>
@@ -1709,11 +1709,11 @@
       </c>
       <c r="J9" s="4">
         <f>SummaryTable_Class_wTotals!H7</f>
-        <v>97400</v>
+        <v>113200</v>
       </c>
       <c r="K9" s="38">
         <f>SummaryTable_Class_wTotals!I7</f>
-        <v>70200</v>
+        <v>86000</v>
       </c>
       <c r="L9" s="31">
         <f>SummaryTable_Class_wTotals!J7</f>
@@ -1721,11 +1721,11 @@
       </c>
       <c r="M9" s="4">
         <f>SummaryTable_Class_wTotals!K7</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N9" s="38">
         <f>SummaryTable_Class_wTotals!L7</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
@@ -1739,11 +1739,11 @@
       </c>
       <c r="D10" s="30">
         <f t="shared" si="0"/>
-        <v>1.0447887531229626E-2</v>
+        <v>1.0447887532556465E-2</v>
       </c>
       <c r="E10" s="12">
         <f t="shared" si="1"/>
-        <v>2.4113294207706047E-2</v>
+        <v>2.5127913587265491E-2</v>
       </c>
       <c r="F10" s="29">
         <f>SummaryTable_Class_wTotals!D8</f>
@@ -1763,11 +1763,11 @@
       </c>
       <c r="J10" s="2">
         <f>SummaryTable_Class_wTotals!H8</f>
-        <v>6600</v>
+        <v>9800</v>
       </c>
       <c r="K10" s="37">
         <f>SummaryTable_Class_wTotals!I8</f>
-        <v>6400</v>
+        <v>9600</v>
       </c>
       <c r="L10" s="29">
         <f>SummaryTable_Class_wTotals!J8</f>
@@ -1775,11 +1775,11 @@
       </c>
       <c r="M10" s="2">
         <f>SummaryTable_Class_wTotals!K8</f>
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="N10" s="37">
         <f>SummaryTable_Class_wTotals!L8</f>
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
@@ -1793,11 +1793,11 @@
       </c>
       <c r="D11" s="32">
         <f t="shared" si="0"/>
-        <v>2.9636634360598914E-2</v>
+        <v>2.963663436436265E-2</v>
       </c>
       <c r="E11" s="13">
         <f t="shared" si="1"/>
-        <v>4.8992089818831332E-2</v>
+        <v>5.139283683911313E-2</v>
       </c>
       <c r="F11" s="31">
         <f>SummaryTable_Class_wTotals!D9</f>
@@ -1817,11 +1817,11 @@
       </c>
       <c r="J11" s="4">
         <f>SummaryTable_Class_wTotals!H9</f>
-        <v>15600</v>
+        <v>22400</v>
       </c>
       <c r="K11" s="38">
         <f>SummaryTable_Class_wTotals!I9</f>
-        <v>13500</v>
+        <v>20300</v>
       </c>
       <c r="L11" s="31">
         <f>SummaryTable_Class_wTotals!J9</f>
@@ -1829,11 +1829,11 @@
       </c>
       <c r="M11" s="4">
         <f>SummaryTable_Class_wTotals!K9</f>
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="N11" s="38">
         <f>SummaryTable_Class_wTotals!L9</f>
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -1843,15 +1843,15 @@
       </c>
       <c r="C12" s="29">
         <f>SummaryTable_Class_wTotals!C10</f>
-        <v>18949.018872781799</v>
+        <v>18949.018868162399</v>
       </c>
       <c r="D12" s="30">
         <f t="shared" si="0"/>
-        <v>0.52094420473386793</v>
+        <v>0.52094420467302982</v>
       </c>
       <c r="E12" s="12">
         <f t="shared" si="1"/>
-        <v>0.30109721867823425</v>
+        <v>0.34837976122797043</v>
       </c>
       <c r="F12" s="29">
         <f>SummaryTable_Class_wTotals!D10</f>
@@ -1871,11 +1871,11 @@
       </c>
       <c r="J12" s="2">
         <f>SummaryTable_Class_wTotals!H10</f>
-        <v>114200</v>
+        <v>184600</v>
       </c>
       <c r="K12" s="37">
         <f>SummaryTable_Class_wTotals!I10</f>
-        <v>80900</v>
+        <v>151300</v>
       </c>
       <c r="L12" s="29">
         <f>SummaryTable_Class_wTotals!J10</f>
@@ -1883,11 +1883,11 @@
       </c>
       <c r="M12" s="2">
         <f>SummaryTable_Class_wTotals!K10</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="N12" s="37">
         <f>SummaryTable_Class_wTotals!L10</f>
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
@@ -1901,11 +1901,11 @@
       </c>
       <c r="D13" s="32">
         <f t="shared" si="0"/>
-        <v>2.8142641255754716E-2</v>
+        <v>2.8142641259328721E-2</v>
       </c>
       <c r="E13" s="13">
         <f t="shared" si="1"/>
-        <v>1.2248022454707833E-2</v>
+        <v>1.6145537237066514E-2</v>
       </c>
       <c r="F13" s="31">
         <f>SummaryTable_Class_wTotals!D11</f>
@@ -1925,11 +1925,11 @@
       </c>
       <c r="J13" s="4">
         <f>SummaryTable_Class_wTotals!H11</f>
-        <v>5300</v>
+        <v>9900</v>
       </c>
       <c r="K13" s="38">
         <f>SummaryTable_Class_wTotals!I11</f>
-        <v>3300</v>
+        <v>7900</v>
       </c>
       <c r="L13" s="31">
         <f>SummaryTable_Class_wTotals!J11</f>
@@ -1937,11 +1937,11 @@
       </c>
       <c r="M13" s="4">
         <f>SummaryTable_Class_wTotals!K11</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="N13" s="38">
         <f>SummaryTable_Class_wTotals!L11</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
@@ -1955,11 +1955,11 @@
       </c>
       <c r="D14" s="30">
         <f t="shared" si="0"/>
-        <v>8.1788393087445357E-2</v>
+        <v>8.178839309783216E-2</v>
       </c>
       <c r="E14" s="12">
         <f t="shared" si="1"/>
-        <v>2.5516713447307986E-2</v>
+        <v>3.4223990903922683E-2</v>
       </c>
       <c r="F14" s="29">
         <f>SummaryTable_Class_wTotals!D12</f>
@@ -1979,11 +1979,11 @@
       </c>
       <c r="J14" s="2">
         <f>SummaryTable_Class_wTotals!H12</f>
-        <v>15400</v>
+        <v>25500</v>
       </c>
       <c r="K14" s="37">
         <f>SummaryTable_Class_wTotals!I12</f>
-        <v>7200</v>
+        <v>17300</v>
       </c>
       <c r="L14" s="29">
         <f>SummaryTable_Class_wTotals!J12</f>
@@ -1991,11 +1991,11 @@
       </c>
       <c r="M14" s="2">
         <f>SummaryTable_Class_wTotals!K12</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="N14" s="37">
         <f>SummaryTable_Class_wTotals!L12</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -2004,7 +2004,7 @@
       </c>
       <c r="C15" s="33">
         <f>SummaryTable_Class_wTotals!C13</f>
-        <v>36374.373110575601</v>
+        <v>36374.373105956198</v>
       </c>
       <c r="D15" s="34">
         <f t="shared" si="0"/>
@@ -2032,11 +2032,11 @@
       </c>
       <c r="J15" s="39">
         <f>SummaryTable_Class_wTotals!H13</f>
-        <v>341800</v>
+        <v>437500</v>
       </c>
       <c r="K15" s="40">
         <f>SummaryTable_Class_wTotals!I13</f>
-        <v>257800</v>
+        <v>353500</v>
       </c>
       <c r="L15" s="33">
         <f>SummaryTable_Class_wTotals!J13</f>
@@ -2044,18 +2044,18 @@
       </c>
       <c r="M15" s="39">
         <f>SummaryTable_Class_wTotals!K13</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="N15" s="40">
         <f>SummaryTable_Class_wTotals!L13</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="46" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="48" t="s">
@@ -2064,27 +2064,27 @@
       <c r="E18" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="45" t="s">
+      <c r="F18" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="46"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="45" t="s">
+      <c r="G18" s="42"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="J18" s="46"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="45" t="s">
+      <c r="J18" s="42"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="46"/>
-      <c r="N18" s="47"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="43"/>
     </row>
     <row r="19" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="44"/>
-      <c r="C19" s="42"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="49"/>
-      <c r="E19" s="44"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="35" t="s">
         <v>7</v>
       </c>
@@ -2123,11 +2123,11 @@
       </c>
       <c r="D20" s="30">
         <f>C20/$C$15</f>
-        <v>2.5662834587113149E-2</v>
+        <v>2.5662834590372229E-2</v>
       </c>
       <c r="E20" s="12">
         <f>(H20+K20)/($H$15+$K$15)</f>
-        <v>0.18716509313600407</v>
+        <v>0.14951677089255258</v>
       </c>
       <c r="F20" s="29">
         <f t="shared" ref="F20:K20" si="2">F4+F5+F6</f>
@@ -2147,11 +2147,11 @@
       </c>
       <c r="J20" s="2">
         <f t="shared" si="2"/>
-        <v>56200</v>
+        <v>41000</v>
       </c>
       <c r="K20" s="37">
         <f t="shared" si="2"/>
-        <v>49800</v>
+        <v>34600</v>
       </c>
       <c r="L20" s="29">
         <f>(F20+I20)/$C20</f>
@@ -2159,11 +2159,11 @@
       </c>
       <c r="M20" s="2">
         <f t="shared" ref="M20:N20" si="3">(G20+J20)/$C20</f>
-        <v>242.96454791130108</v>
+        <v>226.68120960331265</v>
       </c>
       <c r="N20" s="37">
         <f t="shared" si="3"/>
-        <v>157.15564011723046</v>
+        <v>140.87230180924203</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -2176,11 +2176,11 @@
       </c>
       <c r="D21" s="32">
         <f t="shared" ref="D21:D24" si="4">C21/$C$15</f>
-        <v>0.30337740444398964</v>
+        <v>0.30337740448251738</v>
       </c>
       <c r="E21" s="13">
         <f>(H21+K21)/($H$15+$K$15)</f>
-        <v>0.40086756825720848</v>
+        <v>0.37521318931210917</v>
       </c>
       <c r="F21" s="31">
         <f t="shared" ref="F21:K21" si="5">F7+F8+F9</f>
@@ -2200,11 +2200,11 @@
       </c>
       <c r="J21" s="4">
         <f t="shared" si="5"/>
-        <v>128600</v>
+        <v>144400</v>
       </c>
       <c r="K21" s="38">
         <f t="shared" si="5"/>
-        <v>96800</v>
+        <v>112600</v>
       </c>
       <c r="L21" s="31">
         <f t="shared" ref="L21:L23" si="6">(F21+I21)/$C21</f>
@@ -2212,11 +2212,11 @@
       </c>
       <c r="M21" s="4">
         <f t="shared" ref="M21:M23" si="7">(G21+J21)/$C21</f>
-        <v>48.716997179543711</v>
+        <v>50.148783927007983</v>
       </c>
       <c r="N21" s="38">
         <f t="shared" ref="N21:N23" si="8">(H21+K21)/$C21</f>
-        <v>28.472620003371716</v>
+        <v>29.904406750835985</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
@@ -2225,15 +2225,15 @@
       </c>
       <c r="C22" s="29">
         <f>C10+C11+C12</f>
-        <v>20407.068228034204</v>
+        <v>20407.068223414804</v>
       </c>
       <c r="D22" s="30">
         <f t="shared" si="4"/>
-        <v>0.56102872662569647</v>
+        <v>0.56102872656994895</v>
       </c>
       <c r="E22" s="12">
         <f t="shared" ref="E22:E24" si="9">(H22+K22)/($H$15+$K$15)</f>
-        <v>0.37420260270477163</v>
+        <v>0.42490051165434906</v>
       </c>
       <c r="F22" s="29">
         <f t="shared" ref="F22:K22" si="10">F10+F11+F12</f>
@@ -2253,23 +2253,23 @@
       </c>
       <c r="J22" s="2">
         <f t="shared" si="10"/>
-        <v>136400</v>
+        <v>216800</v>
       </c>
       <c r="K22" s="37">
         <f t="shared" si="10"/>
-        <v>100800</v>
+        <v>181200</v>
       </c>
       <c r="L22" s="29">
         <f t="shared" si="6"/>
-        <v>10.417958994616425</v>
+        <v>10.417958996974662</v>
       </c>
       <c r="M22" s="2">
         <f t="shared" si="7"/>
-        <v>24.790430175806438</v>
+        <v>28.730241580085817</v>
       </c>
       <c r="N22" s="37">
         <f t="shared" si="8"/>
-        <v>14.372471181190015</v>
+        <v>18.312282583111156</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -2282,11 +2282,11 @@
       </c>
       <c r="D23" s="32">
         <f t="shared" si="4"/>
-        <v>0.10993103434320008</v>
+        <v>0.10993103435716088</v>
       </c>
       <c r="E23" s="13">
         <f t="shared" si="9"/>
-        <v>3.7764735902015824E-2</v>
+        <v>5.0369528140989196E-2</v>
       </c>
       <c r="F23" s="31">
         <f t="shared" ref="F23:K23" si="11">F13+F14</f>
@@ -2306,11 +2306,11 @@
       </c>
       <c r="J23" s="4">
         <f t="shared" si="11"/>
-        <v>20700</v>
+        <v>35400</v>
       </c>
       <c r="K23" s="38">
         <f t="shared" si="11"/>
-        <v>10500</v>
+        <v>25200</v>
       </c>
       <c r="L23" s="31">
         <f t="shared" si="6"/>
@@ -2318,11 +2318,11 @@
       </c>
       <c r="M23" s="4">
         <f t="shared" si="7"/>
-        <v>20.381764403759057</v>
+        <v>24.057984486400258</v>
       </c>
       <c r="N23" s="38">
         <f t="shared" si="8"/>
-        <v>7.4024567650462334</v>
+        <v>11.078676847687438</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="C24" s="33">
         <f>C15</f>
-        <v>36374.373110575601</v>
+        <v>36374.373105956198</v>
       </c>
       <c r="D24" s="34">
         <f t="shared" si="4"/>
@@ -2359,11 +2359,11 @@
       </c>
       <c r="J24" s="39">
         <f t="shared" si="12"/>
-        <v>341800</v>
+        <v>437500</v>
       </c>
       <c r="K24" s="40">
         <f t="shared" si="12"/>
-        <v>257800</v>
+        <v>353500</v>
       </c>
       <c r="L24" s="33">
         <f t="shared" si="12"/>
@@ -2371,18 +2371,18 @@
       </c>
       <c r="M24" s="39">
         <f t="shared" si="12"/>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="N24" s="40">
         <f t="shared" si="12"/>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="46" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="48" t="s">
@@ -2391,27 +2391,27 @@
       <c r="E27" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="45" t="s">
+      <c r="F27" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="46"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="45" t="s">
+      <c r="G27" s="42"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="46"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="45" t="s">
+      <c r="J27" s="42"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="46"/>
-      <c r="N27" s="47"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="43"/>
     </row>
     <row r="28" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="44"/>
-      <c r="C28" s="42"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="47"/>
       <c r="D28" s="49"/>
-      <c r="E28" s="44"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="35" t="s">
         <v>7</v>
       </c>
@@ -2450,11 +2450,11 @@
       </c>
       <c r="D29" s="30">
         <f>C29/$C$15</f>
-        <v>7.439372792953021E-2</v>
+        <v>7.439372793897793E-2</v>
       </c>
       <c r="E29" s="12">
         <f>(H29+K29)/($H$15+$K$15)</f>
-        <v>0.1878030109721868</v>
+        <v>0.1679363274587834</v>
       </c>
       <c r="F29" s="29">
         <f t="shared" ref="F29:K29" si="13">F4+F7+F10+F13</f>
@@ -2474,11 +2474,11 @@
       </c>
       <c r="J29" s="2">
         <f t="shared" si="13"/>
-        <v>54600</v>
+        <v>55100</v>
       </c>
       <c r="K29" s="37">
         <f t="shared" si="13"/>
-        <v>49800</v>
+        <v>50300</v>
       </c>
       <c r="L29" s="29">
         <f>(F29+I29)/$C29</f>
@@ -2486,11 +2486,11 @@
       </c>
       <c r="M29" s="2">
         <f t="shared" ref="M29:M31" si="14">(G29+J29)/$C29</f>
-        <v>68.587683088850667</v>
+        <v>68.77245594199951</v>
       </c>
       <c r="N29" s="37">
         <f t="shared" ref="N29:N31" si="15">(H29+K29)/$C29</f>
-        <v>54.397127967019493</v>
+        <v>54.581900820168336</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
@@ -2503,11 +2503,11 @@
       </c>
       <c r="D30" s="32">
         <f t="shared" ref="D30:D32" si="16">C30/$C$15</f>
-        <v>0.1366914865157601</v>
+        <v>0.13669148653311938</v>
       </c>
       <c r="E30" s="13">
         <f>(H30+K30)/($H$15+$K$15)</f>
-        <v>0.1747894871140597</v>
+        <v>0.1679363274587834</v>
       </c>
       <c r="F30" s="31">
         <f t="shared" ref="F30:K30" si="17">F5+F8+F11+F14</f>
@@ -2527,11 +2527,11 @@
       </c>
       <c r="J30" s="4">
         <f t="shared" si="17"/>
-        <v>64000</v>
+        <v>74700</v>
       </c>
       <c r="K30" s="38">
         <f t="shared" si="17"/>
-        <v>47600</v>
+        <v>58300</v>
       </c>
       <c r="L30" s="31">
         <f t="shared" ref="L30:L31" si="18">(F30+I30)/$C30</f>
@@ -2539,11 +2539,11 @@
       </c>
       <c r="M30" s="4">
         <f t="shared" si="14"/>
-        <v>54.806178756140824</v>
+        <v>56.958201188033328</v>
       </c>
       <c r="N30" s="38">
         <f t="shared" si="15"/>
-        <v>27.553932071894653</v>
+        <v>29.705954503787154</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
@@ -2552,15 +2552,15 @@
       </c>
       <c r="C31" s="29">
         <f>C6+C9+C12</f>
-        <v>28696.280762216727</v>
+        <v>28696.280757597327</v>
       </c>
       <c r="D31" s="30">
         <f t="shared" si="16"/>
-        <v>0.78891478555470906</v>
+        <v>0.78891478552790217</v>
       </c>
       <c r="E31" s="12">
         <f t="shared" ref="E31:E32" si="19">(H31+K31)/($H$15+$K$15)</f>
-        <v>0.6374075019137535</v>
+        <v>0.66412734508243321</v>
       </c>
       <c r="F31" s="29">
         <f t="shared" ref="F31:K31" si="20">F6+F9+F12</f>
@@ -2580,23 +2580,23 @@
       </c>
       <c r="J31" s="2">
         <f t="shared" si="20"/>
-        <v>223300</v>
+        <v>307800</v>
       </c>
       <c r="K31" s="37">
         <f t="shared" si="20"/>
-        <v>160500</v>
+        <v>245000</v>
       </c>
       <c r="L31" s="29">
         <f t="shared" si="18"/>
-        <v>13.733487041947821</v>
+        <v>13.733487044158577</v>
       </c>
       <c r="M31" s="2">
         <f t="shared" si="14"/>
-        <v>31.143408701823823</v>
+        <v>34.088041173803404</v>
       </c>
       <c r="N31" s="37">
         <f t="shared" si="15"/>
-        <v>17.409921659876002</v>
+        <v>20.354554129644825</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="C32" s="33">
         <f>C24</f>
-        <v>36374.373110575601</v>
+        <v>36374.373105956198</v>
       </c>
       <c r="D32" s="34">
         <f t="shared" si="16"/>
@@ -2633,11 +2633,11 @@
       </c>
       <c r="J32" s="39">
         <f t="shared" si="21"/>
-        <v>341800</v>
+        <v>437500</v>
       </c>
       <c r="K32" s="40">
         <f t="shared" si="21"/>
-        <v>257800</v>
+        <v>353500</v>
       </c>
       <c r="L32" s="33">
         <f t="shared" si="21"/>
@@ -2645,15 +2645,22 @@
       </c>
       <c r="M32" s="39">
         <f t="shared" si="21"/>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="N32" s="40">
         <f t="shared" si="21"/>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="L18:N18"/>
     <mergeCell ref="B27:B28"/>
@@ -2668,13 +2675,6 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="F18:H18"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2685,7 +2685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF95D237-0CC0-48D9-B8E7-CC6B51F60950}">
   <dimension ref="B2:K15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2699,10 +2699,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="44" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="51" t="s">
@@ -2723,9 +2723,9 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="42"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="25" t="s">
         <v>33</v>
       </c>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="D4" s="18">
         <f>C4/$C$15</f>
-        <v>6.8933482387297197E-3</v>
+        <v>6.8933482396051479E-3</v>
       </c>
       <c r="E4" s="6">
         <f>SummaryTable_Class_wTotals!M2</f>
@@ -2783,11 +2783,11 @@
       </c>
       <c r="J4" s="6">
         <f>SummaryTable_Class_wTotals!R2</f>
-        <v>0.52980789576932397</v>
+        <v>0.52945967978247999</v>
       </c>
       <c r="K4" s="7">
         <f>SummaryTable_Class_wTotals!S2</f>
-        <v>0.47019210423067498</v>
+        <v>0.47054032021751901</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="D5" s="19">
         <f t="shared" ref="D5:D15" si="0">C5/$C$15</f>
-        <v>1.0536352038936632E-2</v>
+        <v>1.0536352040274708E-2</v>
       </c>
       <c r="E5" s="8">
         <f>SummaryTable_Class_wTotals!M3</f>
@@ -2825,11 +2825,11 @@
       </c>
       <c r="J5" s="8">
         <f>SummaryTable_Class_wTotals!R3</f>
-        <v>0.266320237231221</v>
+        <v>0.26623302680727101</v>
       </c>
       <c r="K5" s="9">
         <f>SummaryTable_Class_wTotals!S3</f>
-        <v>0.733679762768779</v>
+        <v>0.73376697319272799</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="D6" s="18">
         <f t="shared" si="0"/>
-        <v>8.2331343094467976E-3</v>
+        <v>8.2331343104923727E-3</v>
       </c>
       <c r="E6" s="6">
         <f>SummaryTable_Class_wTotals!M4</f>
@@ -2867,11 +2867,11 @@
       </c>
       <c r="J6" s="6">
         <f>SummaryTable_Class_wTotals!R4</f>
-        <v>0.65618141578857603</v>
+        <v>0.65569806699541899</v>
       </c>
       <c r="K6" s="7">
         <f>SummaryTable_Class_wTotals!S4</f>
-        <v>0.34381858421142297</v>
+        <v>0.34430193300458001</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="D7" s="19">
         <f t="shared" si="0"/>
-        <v>2.8909850903816151E-2</v>
+        <v>2.8909850907487589E-2</v>
       </c>
       <c r="E7" s="8">
         <f>SummaryTable_Class_wTotals!M5</f>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="D8" s="18">
         <f t="shared" si="0"/>
-        <v>1.4730107028779206E-2</v>
+        <v>1.4730107030649872E-2</v>
       </c>
       <c r="E8" s="6">
         <f>SummaryTable_Class_wTotals!M6</f>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="D9" s="19">
         <f t="shared" si="0"/>
-        <v>0.2597374465113943</v>
+        <v>0.25973744654437997</v>
       </c>
       <c r="E9" s="8">
         <f>SummaryTable_Class_wTotals!M7</f>
@@ -2993,11 +2993,11 @@
       </c>
       <c r="J9" s="8">
         <f>SummaryTable_Class_wTotals!R7</f>
-        <v>0.17301672768186099</v>
+        <v>0.17531217444554401</v>
       </c>
       <c r="K9" s="9">
         <f>SummaryTable_Class_wTotals!S7</f>
-        <v>0.82698327231813795</v>
+        <v>0.82468782555445497</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="D10" s="18">
         <f t="shared" si="0"/>
-        <v>1.0447887531229626E-2</v>
+        <v>1.0447887532556465E-2</v>
       </c>
       <c r="E10" s="6">
         <f>SummaryTable_Class_wTotals!M8</f>
@@ -3035,11 +3035,11 @@
       </c>
       <c r="J10" s="6">
         <f>SummaryTable_Class_wTotals!R8</f>
-        <v>6.0419253513439498E-2</v>
+        <v>6.0709244901510098E-2</v>
       </c>
       <c r="K10" s="7">
         <f>SummaryTable_Class_wTotals!S8</f>
-        <v>0.93958074648655998</v>
+        <v>0.93929075509848903</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="D11" s="19">
         <f t="shared" si="0"/>
-        <v>2.9636634360598914E-2</v>
+        <v>2.963663436436265E-2</v>
       </c>
       <c r="E11" s="8">
         <f>SummaryTable_Class_wTotals!M9</f>
@@ -3077,11 +3077,11 @@
       </c>
       <c r="J11" s="8">
         <f>SummaryTable_Class_wTotals!R9</f>
-        <v>0.295774626111724</v>
+        <v>0.29802133716613</v>
       </c>
       <c r="K11" s="9">
         <f>SummaryTable_Class_wTotals!S9</f>
-        <v>0.704225373888275</v>
+        <v>0.701978662833869</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -3091,39 +3091,39 @@
       </c>
       <c r="C12" s="15">
         <f>SummaryTable_Class_wTotals!C10</f>
-        <v>18949.018872781799</v>
+        <v>18949.018868162399</v>
       </c>
       <c r="D12" s="18">
         <f t="shared" si="0"/>
-        <v>0.52094420473386793</v>
+        <v>0.52094420467302982</v>
       </c>
       <c r="E12" s="6">
         <f>SummaryTable_Class_wTotals!M10</f>
-        <v>0.61181353306202302</v>
+        <v>0.61181353296450403</v>
       </c>
       <c r="F12" s="3">
         <f>SummaryTable_Class_wTotals!N10</f>
-        <v>4.9696302055415899E-2</v>
+        <v>4.9696302070419501E-2</v>
       </c>
       <c r="G12" s="7">
         <f>SummaryTable_Class_wTotals!O10</f>
-        <v>0.33849016488256001</v>
+        <v>0.338490164965076</v>
       </c>
       <c r="H12" s="6">
         <f>SummaryTable_Class_wTotals!P10</f>
-        <v>7.6907313903927299E-2</v>
+        <v>7.6907313903587696E-2</v>
       </c>
       <c r="I12" s="7">
         <f>SummaryTable_Class_wTotals!Q10</f>
-        <v>0.92309268609607198</v>
+        <v>0.92309268609641204</v>
       </c>
       <c r="J12" s="6">
         <f>SummaryTable_Class_wTotals!R10</f>
-        <v>0.114978224053234</v>
+        <v>0.121025436355658</v>
       </c>
       <c r="K12" s="7">
         <f>SummaryTable_Class_wTotals!S10</f>
-        <v>0.88502177594676501</v>
+        <v>0.87897456364434101</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -3137,7 +3137,7 @@
       </c>
       <c r="D13" s="19">
         <f t="shared" si="0"/>
-        <v>2.8142641255754716E-2</v>
+        <v>2.8142641259328721E-2</v>
       </c>
       <c r="E13" s="8">
         <f>SummaryTable_Class_wTotals!M11</f>
@@ -3161,11 +3161,11 @@
       </c>
       <c r="J13" s="8">
         <f>SummaryTable_Class_wTotals!R11</f>
-        <v>0.12354183535109101</v>
+        <v>0.130080896644448</v>
       </c>
       <c r="K13" s="9">
         <f>SummaryTable_Class_wTotals!S11</f>
-        <v>0.87645816464890802</v>
+        <v>0.869919103355551</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="D14" s="18">
         <f t="shared" si="0"/>
-        <v>8.1788393087445357E-2</v>
+        <v>8.178839309783216E-2</v>
       </c>
       <c r="E14" s="6">
         <f>SummaryTable_Class_wTotals!M12</f>
@@ -3203,11 +3203,11 @@
       </c>
       <c r="J14" s="6">
         <f>SummaryTable_Class_wTotals!R12</f>
-        <v>0.30025130994892701</v>
+        <v>0.32183997689629801</v>
       </c>
       <c r="K14" s="7">
         <f>SummaryTable_Class_wTotals!S12</f>
-        <v>0.69974869005107199</v>
+        <v>0.67816002310370105</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
@@ -3216,7 +3216,7 @@
       </c>
       <c r="C15" s="17">
         <f>SummaryTable_Class_wTotals!C13</f>
-        <v>36374.373110575601</v>
+        <v>36374.373105956198</v>
       </c>
       <c r="D15" s="20">
         <f t="shared" si="0"/>
@@ -3224,31 +3224,31 @@
       </c>
       <c r="E15" s="10">
         <f>SummaryTable_Class_wTotals!M13</f>
-        <v>0.65372524042376201</v>
+        <v>0.65372524037828295</v>
       </c>
       <c r="F15" s="21">
         <f>SummaryTable_Class_wTotals!N13</f>
-        <v>5.9827875657770799E-2</v>
+        <v>5.9827875666873503E-2</v>
       </c>
       <c r="G15" s="11">
         <f>SummaryTable_Class_wTotals!O13</f>
-        <v>0.28644688391846601</v>
+        <v>0.28644688395484302</v>
       </c>
       <c r="H15" s="10">
         <f>SummaryTable_Class_wTotals!P13</f>
-        <v>0.194119746530757</v>
+        <v>0.19411974653066999</v>
       </c>
       <c r="I15" s="11">
         <f>SummaryTable_Class_wTotals!Q13</f>
-        <v>0.80588025346924197</v>
+        <v>0.80588025346932901</v>
       </c>
       <c r="J15" s="10">
         <f>SummaryTable_Class_wTotals!R13</f>
-        <v>0.22302547624180799</v>
+        <v>0.19540511493389801</v>
       </c>
       <c r="K15" s="11">
         <f>SummaryTable_Class_wTotals!S13</f>
-        <v>0.77697452375819098</v>
+        <v>0.804594885066101</v>
       </c>
     </row>
   </sheetData>
@@ -3270,7 +3270,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:S13"/>
+      <selection activeCell="H11" sqref="A1:S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3361,19 +3361,19 @@
         <v>1000</v>
       </c>
       <c r="H2">
-        <v>22800</v>
+        <v>15500</v>
       </c>
       <c r="I2">
-        <v>21800</v>
+        <v>14500</v>
       </c>
       <c r="J2">
         <v>31</v>
       </c>
       <c r="K2">
-        <v>288</v>
+        <v>259</v>
       </c>
       <c r="L2">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="M2">
         <v>0.56234050665089597</v>
@@ -3391,10 +3391,10 @@
         <v>0.47903200405893598</v>
       </c>
       <c r="R2">
-        <v>0.52980789576932397</v>
+        <v>0.52945967978247999</v>
       </c>
       <c r="S2">
-        <v>0.47019210423067498</v>
+        <v>0.47054032021751901</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -3420,19 +3420,19 @@
         <v>3100</v>
       </c>
       <c r="H3">
-        <v>21700</v>
+        <v>15500</v>
       </c>
       <c r="I3">
-        <v>18600</v>
+        <v>12400</v>
       </c>
       <c r="J3">
         <v>153</v>
       </c>
       <c r="K3">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="L3">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="M3">
         <v>0.75610786350745396</v>
@@ -3450,10 +3450,10 @@
         <v>0.747471798505142</v>
       </c>
       <c r="R3">
-        <v>0.266320237231221</v>
+        <v>0.26623302680727101</v>
       </c>
       <c r="S3">
-        <v>0.733679762768779</v>
+        <v>0.73376697319272799</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -3479,19 +3479,19 @@
         <v>2300</v>
       </c>
       <c r="H4">
-        <v>11700</v>
+        <v>10000</v>
       </c>
       <c r="I4">
-        <v>9400</v>
+        <v>7700</v>
       </c>
       <c r="J4">
         <v>46</v>
       </c>
       <c r="K4">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="L4">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="M4">
         <v>0.64887076252914699</v>
@@ -3509,10 +3509,10 @@
         <v>0.36656462875153001</v>
       </c>
       <c r="R4">
-        <v>0.65618141578857603</v>
+        <v>0.65569806699541899</v>
       </c>
       <c r="S4">
-        <v>0.34381858421142297</v>
+        <v>0.34430193300458001</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -3656,19 +3656,19 @@
         <v>27200</v>
       </c>
       <c r="H7">
-        <v>97400</v>
+        <v>113200</v>
       </c>
       <c r="I7">
-        <v>70200</v>
+        <v>86000</v>
       </c>
       <c r="J7">
         <v>19</v>
       </c>
       <c r="K7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M7">
         <v>0.73807658061037795</v>
@@ -3686,10 +3686,10 @@
         <v>0.83773955733911498</v>
       </c>
       <c r="R7">
-        <v>0.17301672768186099</v>
+        <v>0.17531217444554401</v>
       </c>
       <c r="S7">
-        <v>0.82698327231813795</v>
+        <v>0.82468782555445497</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -3715,19 +3715,19 @@
         <v>200</v>
       </c>
       <c r="H8">
-        <v>6600</v>
+        <v>9800</v>
       </c>
       <c r="I8">
-        <v>6400</v>
+        <v>9600</v>
       </c>
       <c r="J8">
         <v>4</v>
       </c>
       <c r="K8">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L8">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="M8">
         <v>0.341768083148071</v>
@@ -3745,10 +3745,10 @@
         <v>0.96285435581591905</v>
       </c>
       <c r="R8">
-        <v>6.0419253513439498E-2</v>
+        <v>6.0709244901510098E-2</v>
       </c>
       <c r="S8">
-        <v>0.93958074648655998</v>
+        <v>0.93929075509848903</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -3774,19 +3774,19 @@
         <v>2100</v>
       </c>
       <c r="H9">
-        <v>15600</v>
+        <v>22400</v>
       </c>
       <c r="I9">
-        <v>13500</v>
+        <v>20300</v>
       </c>
       <c r="J9">
         <v>13</v>
       </c>
       <c r="K9">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L9">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="M9">
         <v>0.50580354474710199</v>
@@ -3804,10 +3804,10 @@
         <v>0.76119876590687796</v>
       </c>
       <c r="R9">
-        <v>0.295774626111724</v>
+        <v>0.29802133716613</v>
       </c>
       <c r="S9">
-        <v>0.704225373888275</v>
+        <v>0.701978662833869</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -3818,7 +3818,7 @@
         <v>44</v>
       </c>
       <c r="C10">
-        <v>18949.018872781799</v>
+        <v>18949.018868162399</v>
       </c>
       <c r="D10">
         <v>163200</v>
@@ -3833,40 +3833,40 @@
         <v>33300</v>
       </c>
       <c r="H10">
-        <v>114200</v>
+        <v>184600</v>
       </c>
       <c r="I10">
-        <v>80900</v>
+        <v>151300</v>
       </c>
       <c r="J10">
         <v>10</v>
       </c>
       <c r="K10">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="L10">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="M10">
-        <v>0.61181353306202302</v>
+        <v>0.61181353296450403</v>
       </c>
       <c r="N10">
-        <v>4.9696302055415899E-2</v>
+        <v>4.9696302070419501E-2</v>
       </c>
       <c r="O10">
-        <v>0.33849016488256001</v>
+        <v>0.338490164965076</v>
       </c>
       <c r="P10">
-        <v>7.6907313903927299E-2</v>
+        <v>7.6907313903587696E-2</v>
       </c>
       <c r="Q10">
-        <v>0.92309268609607198</v>
+        <v>0.92309268609641204</v>
       </c>
       <c r="R10">
-        <v>0.114978224053234</v>
+        <v>0.121025436355658</v>
       </c>
       <c r="S10">
-        <v>0.88502177594676501</v>
+        <v>0.87897456364434101</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -3892,19 +3892,19 @@
         <v>2000</v>
       </c>
       <c r="H11">
-        <v>5300</v>
+        <v>9900</v>
       </c>
       <c r="I11">
-        <v>3300</v>
+        <v>7900</v>
       </c>
       <c r="J11">
         <v>6</v>
       </c>
       <c r="K11">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L11">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="M11">
         <v>0.63009872257295896</v>
@@ -3922,10 +3922,10 @@
         <v>0.93190123518479195</v>
       </c>
       <c r="R11">
-        <v>0.12354183535109101</v>
+        <v>0.130080896644448</v>
       </c>
       <c r="S11">
-        <v>0.87645816464890802</v>
+        <v>0.869919103355551</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -3951,19 +3951,19 @@
         <v>8200</v>
       </c>
       <c r="H12">
-        <v>15400</v>
+        <v>25500</v>
       </c>
       <c r="I12">
-        <v>7200</v>
+        <v>17300</v>
       </c>
       <c r="J12">
         <v>15</v>
       </c>
       <c r="K12">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L12">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="M12">
         <v>0.71715067020525403</v>
@@ -3981,10 +3981,10 @@
         <v>0.78686229756453696</v>
       </c>
       <c r="R12">
-        <v>0.30025130994892701</v>
+        <v>0.32183997689629801</v>
       </c>
       <c r="S12">
-        <v>0.69974869005107199</v>
+        <v>0.67816002310370105</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -3992,7 +3992,7 @@
         <v>66</v>
       </c>
       <c r="C13">
-        <v>36374.373110575601</v>
+        <v>36374.373105956198</v>
       </c>
       <c r="D13">
         <v>483900</v>
@@ -4007,40 +4007,40 @@
         <v>84000</v>
       </c>
       <c r="H13">
-        <v>341800</v>
+        <v>437500</v>
       </c>
       <c r="I13">
-        <v>257800</v>
+        <v>353500</v>
       </c>
       <c r="J13">
         <v>16</v>
       </c>
       <c r="K13">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L13">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="M13">
-        <v>0.65372524042376201</v>
+        <v>0.65372524037828295</v>
       </c>
       <c r="N13">
-        <v>5.9827875657770799E-2</v>
+        <v>5.9827875666873503E-2</v>
       </c>
       <c r="O13">
-        <v>0.28644688391846601</v>
+        <v>0.28644688395484302</v>
       </c>
       <c r="P13">
-        <v>0.194119746530757</v>
+        <v>0.19411974653066999</v>
       </c>
       <c r="Q13">
-        <v>0.80588025346924197</v>
+        <v>0.80588025346932901</v>
       </c>
       <c r="R13">
-        <v>0.22302547624180799</v>
+        <v>0.19540511493389801</v>
       </c>
       <c r="S13">
-        <v>0.77697452375819098</v>
+        <v>0.804594885066101</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>